<commit_message>
Manual testcases added in supplierhub
</commit_message>
<xml_diff>
--- a/Testcases_supplier/Directory/Manual testcases/Directory listing testcases.xlsx
+++ b/Testcases_supplier/Directory/Manual testcases/Directory listing testcases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Testcases_supplier\Directory\Manual testcases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Zeemart All\Git hub\zm-buyerautomation\Testcases_supplier\Directory\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81D3AE6-CBA0-425A-9BFA-197E5717CF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E476C79-6AFD-45B3-BE4B-3BBEFDBD48B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="69">
   <si>
     <t>SL. No</t>
   </si>
@@ -1109,6 +1109,126 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> , it displayed Deleted successfully</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Click the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 'Your listing is live'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It should have </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'URL'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> options</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If click </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">URL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,it displayed banner items</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If click </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">URL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,it displayed banner items,we replace it with the purple “Buy Now, Pay Later! At zero costs“ banner that currently appears on the homepage . Both desktop and mobile version of the directory</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If click </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">URL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,it displayed banner items,we added For the desktop version, we may need to define a background colour that extends from the sides of the banner: #4132c0</t>
     </r>
   </si>
 </sst>
@@ -1162,7 +1282,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1185,22 +1305,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1209,18 +1318,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1503,10 +1609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,12 +1668,13 @@
       <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -1585,12 +1692,13 @@
       <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -1608,15 +1716,16 @@
       <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1634,12 +1743,13 @@
       <c r="F5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1657,12 +1767,13 @@
       <c r="F6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1680,12 +1791,13 @@
       <c r="F7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1703,12 +1815,13 @@
       <c r="F8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1726,12 +1839,13 @@
       <c r="F9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1749,12 +1863,13 @@
       <c r="F10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1772,12 +1887,13 @@
       <c r="F11" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1795,12 +1911,13 @@
       <c r="F12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1818,12 +1935,13 @@
       <c r="F13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1841,12 +1959,13 @@
       <c r="F14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1864,12 +1983,13 @@
       <c r="F15" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1884,15 +2004,16 @@
       <c r="E16" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="G16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1910,12 +2031,13 @@
       <c r="F17" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="G17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1930,15 +2052,16 @@
       <c r="E18" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="G18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1953,15 +2076,16 @@
       <c r="E19" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G19" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="G19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1976,15 +2100,16 @@
       <c r="E20" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="G20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1999,12 +2124,85 @@
       <c r="E21" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="G21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>